<commit_message>
import de excel a sqlLite
</commit_message>
<xml_diff>
--- a/app/components/File/prueba2.xlsx
+++ b/app/components/File/prueba2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaque\OneDrive\Desktop\Remix\Remix 1\RemixPage\app\components\File\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D00C9D6-8D98-4C5D-AB1E-21964E6A5C6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86EEABC-A2C7-4B44-AD14-035C2F396A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A54FD33-B3AC-4EB9-87A6-1C692C04CC80}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6A54FD33-B3AC-4EB9-87A6-1C692C04CC80}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,43 +20,47 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>edad</t>
-  </si>
-  <si>
-    <t>genero</t>
-  </si>
-  <si>
-    <t>estatura</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Julian 1</t>
   </si>
   <si>
-    <t>hombre</t>
-  </si>
-  <si>
     <t>Julian 2</t>
   </si>
   <si>
-    <t>Julian 3</t>
+    <t>email</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>aaadfs</t>
+  </si>
+  <si>
+    <t>Julian 4</t>
+  </si>
+  <si>
+    <t>datos</t>
+  </si>
+  <si>
+    <t>julian 4</t>
+  </si>
+  <si>
+    <t>sss</t>
   </si>
 </sst>
 </file>
@@ -100,10 +104,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,72 +424,56 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1.22</v>
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1.22</v>
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>1.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>

</xml_diff>